<commit_message>
read excel without sheetread
</commit_message>
<xml_diff>
--- a/read1cell.xlsx
+++ b/read1cell.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\poc\github\oplexcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\poc\github\oplexcel\oplexcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A951529F-CCDE-4F83-AD1A-EBA8BD96068D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C29A3A7-8D1D-485D-AD3D-C6D1D3F03A06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5628" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,17 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>INPUT</t>
+  </si>
+  <si>
+    <t>OUTPUT</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -337,15 +348,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
         <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>